<commit_message>
Added Combiner Functions, Added Bert for 325s. Added resets to trellis for simulation
</commit_message>
<xml_diff>
--- a/stcDemod/Documentation/PilotSyncOffset.xlsx
+++ b/stcDemod/Documentation/PilotSyncOffset.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frank.ziegler\Documents\GitHub\stcDemod\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semco\Vivado\Demods2017\stcDemod\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6A9D4B-BB09-4F85-A3D1-0B9EFE28F91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20955" windowHeight="11235"/>
+    <workbookView xWindow="8160" yWindow="0" windowWidth="16560" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>PilotPulse</t>
   </si>
@@ -103,12 +114,18 @@
   </si>
   <si>
     <t>Calculation time before next packet</t>
+  </si>
+  <si>
+    <t>FFT Latency</t>
+  </si>
+  <si>
+    <t>4892 clocks from start of ValidOut to StartOut</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -462,20 +479,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -483,7 +500,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -509,7 +526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -537,7 +554,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -577,7 +594,7 @@
         <v>-505</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -619,7 +636,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -656,7 +673,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -693,7 +710,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -712,7 +729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -731,7 +748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -751,7 +768,15 @@
         <v>512</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11">
+        <v>3203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -764,7 +789,7 @@
         <v>4858</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -772,7 +797,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14">
         <f>B12-B13</f>
@@ -782,15 +807,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -799,98 +829,129 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>40000000</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19:B24" si="2">(B$27/(A19*1.04)*B$26-B$28)/26</f>
+        <f>(B$29/(A19*1.04)*B$28-B$30)/26</f>
         <v>62.358974358974379</v>
       </c>
       <c r="E19">
         <v>2470</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>30000000</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" si="2"/>
+        <f>(B$29/(A20*1.04)*B$28-B$30)/26</f>
         <v>253.81196581196576</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20000000</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" si="2"/>
+        <f>(B$29/(A21*1.04)*B$28-B$30)/26</f>
         <v>636.71794871794873</v>
       </c>
       <c r="E21">
         <v>1536</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>15000000</v>
+        <v>19000000</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" si="2"/>
-        <v>1019.6239316239315</v>
-      </c>
-      <c r="E22">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B22:B23" si="2">(B$29/(A22*1.04)*B$28-B$30)/26</f>
+        <v>697.17678812415647</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>10000000</v>
+        <v>17000000</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" si="2"/>
+        <v>839.43288084464552</v>
+      </c>
+      <c r="H23">
+        <v>1220</v>
+      </c>
+      <c r="I23">
+        <v>891</v>
+      </c>
+      <c r="J23">
+        <f>H23-I23</f>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>15000000</v>
+      </c>
+      <c r="B24" s="2">
+        <f>(B$29/(A24*1.04)*B$28-B$30)/26</f>
+        <v>1019.6239316239315</v>
+      </c>
+      <c r="E24">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="B25" s="2">
+        <f>(B$29/(A25*1.04)*B$28-B$30)/26</f>
         <v>1785.4358974358975</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <v>1024</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
         <v>5000000</v>
       </c>
-      <c r="B24" s="2">
-        <f t="shared" si="2"/>
+      <c r="B26" s="2">
+        <f>(B$29/(A26*1.04)*B$28-B$30)/26</f>
         <v>4082.8717948717949</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <v>1024</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B28" s="1">
         <f>560000000/3</f>
         <v>186666666.66666666</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>3328</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B28">
-        <f>B27*4</f>
+      <c r="B30">
+        <f>B29*4</f>
         <v>13312</v>
       </c>
     </row>

</xml_diff>